<commit_message>
daily: update naver news outputs
</commit_message>
<xml_diff>
--- a/naver_news_20251027_07to07.report.xlsx
+++ b/naver_news_20251027_07to07.report.xlsx
@@ -8,14 +8,23 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="전체" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 신축" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="신축공사" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 증설" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="증설 공사" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="시설 투자" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="설비투자" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="투자유치" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="투자 유치" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 신설" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 신축" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="신축공사" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 증설" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="생산능력 확대" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 증축" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="증축 공사" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="증축공사" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="라인 증설" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="증설 공사" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="시설 투자" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="설비투자" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="공장 투자" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="신규 투자" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="투자협약" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="투자유치" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="투자 유치" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,239 +503,259 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.48194444444</v>
+        <v>45955.25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
+          <t>[2025 국정감사] “금융사고 최소화…건전성 관리 강화” 촉구</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
+          <t>외부인에 의한 사기 피해 증가 지역 농축협 부실대출 등 지적 농협 유통 자회사 경영개선 방안 마사회 퇴역마 보호·지원 주문 ◆농협 금융 건전성 강화 요구 집중=이날 국감에선 농축협</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>공장 신축, 신축공사</t>
+          <t>공장 신설</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>경북</t>
+          <t>제주</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/662/0000080587?sid=102</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45956.72430555556</v>
+        <v>45954.58819444444</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>인천시 검단6중 신축 현장서 근로자 추락 부상…안전관리 ‘허술’ 지적</t>
+          <t>증평군-코스맥스펫 400억 규모 신규 공장 설립 투자협약</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>인천광역시 서구 불로동 247-16 일원 에서 추진 중인 가칭 ‘검단6중학교 신축공사’ 현장에서 근로자가 추락해 부상을 입는 사고가 발생했다. 공공 발주 대형 건축사업임에도 기본적</t>
+          <t>(증평=뉴스1) 엄기찬 기자 = 충북 증평군은 코스맥스펫㈜과 증평2일반산업단지에 신규 공장을 설립하는 내용의 투자협약을 했다고 24일 밝혔다. 코스맥스펫은 세계 1위 OEM·ODM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>신축공사</t>
+          <t>투자협약</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>400</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>인천광역시 서구 불로동</t>
+          <t>충북 증평군</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/382/0001231641?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008560369?sid=102</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45956.61388888889</v>
+        <v>45954.5875</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>속초시의회, 2025년도 주요사업장 현지답사 실시</t>
+          <t>코스맥스펫, 증평2산단 '반려동물 건강식품 공장 ' 설립한다</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>속초시의회, 2025년도 주요사업장 현지답사 실시 이번 현지답사는 속초영어도서관 신축공사, 속초시 장애인종합복지센터 조성사업, 속초음식문화복합공간 조성사업 등 시민들의 삶의 질 향</t>
+          <t>[증평=뉴시스] 서주영 기자 = 충북 증평군은 지난 23일 김득신문학관에서 코스맥스펫과 지역 신규 공장을 설립하는 투자협약(MOU)을 체결했다고 24일 밝혔다. 코스맥스펫은 400</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>신축공사</t>
+          <t>투자협약</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>충북 증평군</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/087/0001150407?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013555919?sid=102</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45957.12638888889</v>
+        <v>45954.25069444445</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
+          <t>"한국판 ASML 필요"…소부장 핵심전략지도 만든다[Pick코노미]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
+          <t>고부가·탄소중립·핵심광물 등 4대 혁신기술 R&amp;D 역량 집중 15대 프로젝트에 3000억 투자 "첨단산업 기술 수준 83.3점서 2030년 92점까지 끌어올릴것" [서울경제] 정부</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>공장 증설, 증설 공사</t>
+          <t>공장 신설</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/011/0004547151?sid=101</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45956.78541666667</v>
+        <v>45956.48194444444</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산</t>
+          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산 美공장 증설·공급망 재편으로 돌파 넥센, 15%로 완화시 큰 수혜 전망 미국의 관세 폭탄으로 올해 3·4분기 한국타이어앤</t>
+          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>공장 신축, 신축공사</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>경북</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/014/0005424711?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45956.67847222222</v>
+        <v>45954.725</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>타이어 3사 3분기 관세 손실 1150억대…공급망 재편으로 돌파구 모색</t>
+          <t>이노테크, 공모가 1만4700원 확정</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">관세 피해에 공급망 재편·가격 인상 대응 관세 15% 인하 시나리오에 업계 기대감 한국타이어의 미국 테네시 공장 전경.사진=한국타이어앤테크놀로지 제공 [파이낸셜뉴스] 미국의 관세 </t>
+          <t>11월 7일 코스닥 상장 예정복합 신뢰성 환경시험 장비 전문 기업 이노테크가 공모가를 희망가 상단인 1만 4700원으로 확정했다. 24일 금융투자업계에 따르면 이노테크는 지난 22</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>공장 신축</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>259</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/014/0005424606?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/031/0000974916?sid=101</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45956.48541666667</v>
+        <v>45954.66875</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹 "美 테네시 주지사와 공동협력 논의"</t>
+          <t>"매년 30명 사망"…정부, 내년부터 지붕공사 사고 예방·감독 강화</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[서울=뉴시스] 류인선 기자 = 한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 경기 판교 본사 테크노플렉스를 방문해 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴</t>
+          <t>건설업 사망 10%가 지붕공사…봄·가을철 발생 많아 내년부터 대대적 캠페인 후 집중감독…위법 엄중 조치 2027년부터는 건설업 등록업체만 지붕공사 가능 [서울=뉴시스] 고홍주 기자</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013557923?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013556331?sid=102</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45956.48263888889</v>
+        <v>45954.53541666667</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동…“협력 강화 논의”</t>
+          <t>조현준 효성그룹 회장 "글로벌 수요 대응 위해선 생산능력 확보 필수"</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 오전 경기도 판교 본사 테크노플렉스를 방문했다고 26일 밝혔다. 리 주지사는 테크노플렉스를 둘러보고, 이수일 부회장 겸 </t>
+          <t xml:space="preserve">조현준 효성그룹 회장 "글로벌 수요 대응 위해선 생산능력 확보 필수" 효성중공업이 국내외 생산거점 가동률 역대 최고 수준을 기록하며 '글로벌 전력기기 시장'에서 존재감을 강화하고 </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -735,65 +764,77 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2071</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>경기도</t>
+          <t>경남</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/029/0002989234?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/047/0002492510?sid=100</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45956.47916666666</v>
+        <v>45956.72430555556</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+          <t>인천시 검단6중 신축 현장서 근로자 추락 부상…안전관리 ‘허술’ 지적</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>양측은 간담회에서 ▲비즈니스 친화적 환경 조성 ▲원활한 현지 진출을 위한 주정부 차원의 지원 ▲안정적인 에너지 공급 ▲경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+          <t>인천광역시 서구 불로동 247-16 일원 에서 추진 중인 가칭 ‘검단6중학교 신축공사’ 현장에서 근로자가 추락해 부상을 입는 사고가 발생했다. 공공 발주 대형 건축사업임에도 기본적</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>인천광역시 서구 불로동</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005669545?sid=103</t>
+          <t>https://n.news.naver.com/mnews/article/382/0001231641?sid=102</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45956.46388888889</v>
+        <v>45956.61388888889</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 테네시 주지사와 북미 생산·공급망 협력 논의</t>
+          <t>속초시의회, 2025년도 주요사업장 현지답사 실시</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>배터리·타이어 공장 증설 등 북미 생산거점 협력 논의 조현범 회장 강조한 ‘국가 경제 기여’ 실현 의지도 재확인 이날 간담회에는 이수일 한국앤컴퍼니그룹 부회장 겸 한온시스템 대표,</t>
+          <t>속초시의회, 2025년도 주요사업장 현지답사 실시 이번 현지답사는 속초영어도서관 신축공사, 속초시 장애인종합복지센터 조성사업, 속초음식문화복합공간 조성사업 등 시민들의 삶의 질 향</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -802,232 +843,1008 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/119/0003016629?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/087/0001150407?sid=102</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45956.43819444445</v>
+        <v>45956.25</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+          <t>'싱크홀 경고등' 서울 향후 5년간 10m 이상 지하 굴착 공사 300여곳</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>(서울=뉴스1) 박기범 기자 = 빌 리 미국 테네시 주지사와 한국앤컴퍼니(000240)그룹이 미국 내 타이어 생산 확대 및 모빌리티 기술 개발을 위한 협력 방안을 모색했다. 한국앤</t>
+          <t xml:space="preserve">시 "매달 1회 점검…대형 공사 주1회 집중 점검" (서울=뉴스1) 이비슬 기자 = 향후 5년간 서울 전역에서 땅속 10m 이상을 굴착하는 공사 현장이 300여곳에 이르는 것으로 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>증설 공사</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>경기도</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/421/0008562459?sid=103</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008562260?sid=102</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45956.42152777778</v>
+        <v>45955.40694444445</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동… 모빌리티 협력 강화</t>
+          <t>[자막뉴스] " 공사 소리도 좋아"...'3억 달러' 무도회장 착공 논란 파장 ...</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>이번 방문에서 리 주지사는 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴퍼니 대표이사, 김준현 한국앤컴퍼니 경영총괄, 안종선·이상훈 한국타이어앤테크놀로지 공동대표 등을 만났다</t>
+          <t>[자막뉴스] "공사 소리도 좋아"...'3억 달러' 무도회장 착공 논란 파장 계속 수용 인원 999명의 대형 무도회장 신축 공사가 시작됐습니다. [도널드 트럼프 / 미국 대통령 :</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>증축 공사</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>6388</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>02-398-8585</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/366/0001117399?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/052/0002264247?sid=104</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45956.40486111111</v>
+        <v>45955.10138888889</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+          <t>백악관에 '3억 달러' 무도회장 착공...불투명 지적에 트럼프 "3류 기자"</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>간담회에서 양측은 △비즈니스 친화적 환경 조성 △원활한 현지 진출을 위한 주정부 차원의 지원 △안정적인 에너지 공급 △경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+          <t>백악관에 '3억 달러' 무도회장 착공...불투명 지적에 트럼프 "3류 기자" 미국 연방정부의 일시적 업무중지, '셧다운'이 20여 일째 이어지는 가운데 백악관에서는 3억 달러가 들</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>증축 공사</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>02-398-8585</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/008/0005268104?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/052/0002264171?sid=104</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45956.38263888889</v>
+        <v>45954.85833333333</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>“증권사 앱 설치하는 사이에 50만닉스”…다 놓쳤다면 ‘반도체 5총사...</t>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>한미반도체·이수페타시스·ISC등 주목 추석 명절 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사가 없는 투자자들은 ‘포모’(FOMO·기회 상실 걱정)가 커진다</t>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>설비투자</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/009/0005579005?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013556752?sid=100</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45956.42430555556</v>
+        <v>45954.85833333333</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>이번주 공모주 청약, 이노테크 1개사</t>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>27~28일 공모 청약…내달 7일 코스닥 상장 26일 금융투자업계에 따르면, 이노테크는 오는 27~28일 양일간 일반 공모 청약을 실시한다. 앞서 지난 16일부터 22일까지 수요예</t>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>공장 증설</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>259</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/119/0003016600?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013556750?sid=100</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45957.25</v>
+        <v>45954.85833333333</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[S리포트] ②'먹튀의 덫'… 산업 동맥경화 부르는 사모펀드식 경영</t>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"저희는 기업의 가치를 높이는 자본시장의 '메기'입니다." 한때 사모펀드(PEF) 운용사들이 입버릇처럼 하던 말이다. PEF는 본래 저평가된 기업을 인수해 비효율적인 구조를 혁신하</t>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>시설 투자</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/417/0001108955?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013556751?sid=100</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45956.96875</v>
+        <v>45954.85833333333</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>투자유치, 투자 유치</t>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>경기도</t>
+          <t>충남 아산시</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013556753?sid=100</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45957.12638888889</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>공장 증설, 증설 공사</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45956.78541666667</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산 美공장 증설·공급망 재편으로 돌파 넥센, 15%로 완화시 큰 수혜 전망 미국의 관세 폭탄으로 올해 3·4분기 한국타이어앤</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/014/0005424711?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45956.67847222222</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>타이어 3사 3분기 관세 손실 1150억대…공급망 재편으로 돌파구 모색</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관세 피해에 공급망 재편·가격 인상 대응 관세 15% 인하 시나리오에 업계 기대감 한국타이어의 미국 테네시 공장 전경.사진=한국타이어앤테크놀로지 제공 [파이낸셜뉴스] 미국의 관세 </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/014/0005424606?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45956.48541666667</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹 "美 테네시 주지사와 공동협력 논의"</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 류인선 기자 = 한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 경기 판교 본사 테크노플렉스를 방문해 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013557923?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45956.48263888889</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동…“협력 강화 논의”</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 오전 경기도 판교 본사 테크노플렉스를 방문했다고 26일 밝혔다. 리 주지사는 테크노플렉스를 둘러보고, 이수일 부회장 겸 </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/029/0002989234?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45956.47916666666</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>양측은 간담회에서 ▲비즈니스 친화적 환경 조성 ▲원활한 현지 진출을 위한 주정부 차원의 지원 ▲안정적인 에너지 공급 ▲경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/277/0005669545?sid=103</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45956.46388888889</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 테네시 주지사와 북미 생산·공급망 협력 논의</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>배터리·타이어 공장 증설 등 북미 생산거점 협력 논의 조현범 회장 강조한 ‘국가 경제 기여’ 실현 의지도 재확인 이날 간담회에는 이수일 한국앤컴퍼니그룹 부회장 겸 한온시스템 대표,</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/119/0003016629?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45956.43819444445</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>(서울=뉴스1) 박기범 기자 = 빌 리 미국 테네시 주지사와 한국앤컴퍼니(000240)그룹이 미국 내 타이어 생산 확대 및 모빌리티 기술 개발을 위한 협력 방안을 모색했다. 한국앤</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>증설 공사</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008562459?sid=103</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45956.42152777778</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동… 모빌리티 협력 강화</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>이번 방문에서 리 주지사는 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴퍼니 대표이사, 김준현 한국앤컴퍼니 경영총괄, 안종선·이상훈 한국타이어앤테크놀로지 공동대표 등을 만났다</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/366/0001117399?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45956.40486111111</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>간담회에서 양측은 △비즈니스 친화적 환경 조성 △원활한 현지 진출을 위한 주정부 차원의 지원 △안정적인 에너지 공급 △경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/008/0005268104?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45953.35902777778</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>그로쓰리서치 "인벤티지랩, '균일 미립구'로 장기지속형 시장 정조준"</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 배요한 기자 = 인벤티지랩이 미세유체공학 기반의 제형 플랫폼 'IVL-DrugFluidic'을 앞세워 장기지속형(LAI) 의약품 시장 공략에 속도를 내고 있다. 균</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>공장 투자</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013552176?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45952.6875</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>LS일렉, 3분기 영업익 1007억…작년 동기 대비 51.7%↑</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>(서울=뉴스1) 원태성 기자 = LS일렉트릭이 인공지능(AI) 시대 전력기기 호황에 힘입어 3분기 영업이익이 50% 이상 급증하고 매출 역시 20% 가까이 늘어났다. LS일렉트릭은</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>생산능력 확대</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1007</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008555777?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45952.66944444444</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>LS일렉트릭, 실적 훈풍 제대로 탔다…북미 수주 물밀듯</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>북미 매출 비중 33%·5년간 연평균 성장률 50% 달해 자동화 흑자전환·자회사 호조로 수익성 개선세 강화 수주잔고 4.1조 '사상 최대' LS일렉트릭은 올해 3분기 연결기준 매출</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>공장 증축</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2162</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/648/0000040955?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45955.53958333333</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>조승환 의원, 혜광고 다목적강당 증축 …교육부 특별교부금 18.8억 확보</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>(부산=뉴스1) 임순택 기자 = 조승환 국민의힘 의원(부산 중구·영도구)이 부산 혜광고등학교 다목적강당 증축 사업을 위한 교육부 특별교부금 18억 8100만 원을 확보했다고 25일</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>증축 공사, 증축공사</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008561885?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45954.73263888889</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>정부 부채만 38조 달러인데…백악관 뜯어고치는 트럼프</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">'건물 철거 안 해' 약속 파기 정부 계약 체결 기업 기부금 논란 도널드 트럼프 미국 대통령이 추진하는 백악관 증축 공사에 논란이 일고 있다. 1902년 건설된 이스트윙(동관)을 </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>증축 공사</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>1433</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/629/0000437186?sid=104</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45956.38263888889</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>“증권사 앱 설치하는 사이에 50만닉스”…다 놓쳤다면 ‘반도체 5총사...</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>한미반도체·이수페타시스·ISC등 주목 추석 명절 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사가 없는 투자자들은 ‘포모’(FOMO·기회 상실 걱정)가 커진다</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/009/0005579005?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45955.32986111111</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>'아, 포트폴리오 하나쯤 담을 걸'…AI발 훈풍 확산</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>'아, 포트폴리오 하나쯤 담을 걸'…AI발 훈풍 확산 에너지 인프라, 2차전지 관련주에 투자하는 상장지수펀드(ETF)가 이번주 수익률 상위권을 휩쓸었다. 기존 반도체·빅테크 중심으</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2,986</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/215/0001228287?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45954.70555555556</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>9만전자·50만닉스 놓쳤다면 …'K반도체 명품조연' 5총사 주목</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>'반도체 투톱' 말고도 AI 수혜 기업들 있다 "삼성전자, SK하이닉스 없어요?" 추석 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사를 보유하지 않은 투자자</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/009/0005578662?sid=105</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45956.42430555556</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>이번주 공모주 청약, 이노테크 1개사</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>27~28일 공모 청약…내달 7일 코스닥 상장 26일 금융투자업계에 따르면, 이노테크는 오는 27~28일 양일간 일반 공모 청약을 실시한다. 앞서 지난 16일부터 22일까지 수요예</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>259</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/119/0003016600?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45954.47083333333</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>美 테네시 주지사·한국타이어, 현지투자 협력</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>테네시 타이어공장 2조 증설 프로젝트 점검 류진 한경협 회장·이석희 SK온 CEO도 만나 관세 장벽 속 국내 기업과 협력 강화 움직임 6년 만의 방한 일정을 소화 중인 빌 리 테네</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>신규 투자</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>550만</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/016/0002546811?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45954.38819444444</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>[단독] 테네시 주지사, 한국타이어 최고경영진과 ‘장시간 회동’…“한...</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>테네시 타이어공장 2조 증설 프로젝트 점검 ‘관세 장벽’ 속 협력 강화 논의 관측 [헤럴드경제(성남)=김성우 기자] 6년 만의 방한 일정을 소화 중인 빌 리 테네시 주지사가 24일</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>신규 투자</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>550만</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>경기도 성남시</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/016/0002546648?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45954.3875</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>‘비규제 청정지역’ 평택, 삼성전자 P5 착공 호재에 ‘힐스테이트 평택...</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>[서울경제] 정부가 10·15 부동산 대책을 통해 서울과 주요 수도권 지역을 규제지역으로 재지정하면서 실수요자들의 자금 흐름이 바뀌고 있다. 투기과열지구와 조정대상지역 확대로 대출</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>라인 증설, 증설 공사</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>경기도 평택시 합정동</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/011/0004547213?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45957.25</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>[S리포트] ②'먹튀의 덫'… 산업 동맥경화 부르는 사모펀드식 경영</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>"저희는 기업의 가치를 높이는 자본시장의 '메기'입니다." 한때 사모펀드(PEF) 운용사들이 입버릇처럼 하던 말이다. PEF는 본래 저평가된 기업을 인수해 비효율적인 구조를 혁신하</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>시설 투자</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/417/0001108955?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45956.96875</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>투자유치, 투자 유치</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
         <is>
           <t>https://n.news.naver.com/mnews/article/005/0001810151?sid=102</t>
         </is>
@@ -1038,7 +1855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1101,34 +1918,34 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.48194444444</v>
+        <v>45954.3875</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
+          <t>‘비규제 청정지역’ 평택, 삼성전자 P5 착공 호재에 ‘힐스테이트 평택...</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
+          <t>[서울경제] 정부가 10·15 부동산 대책을 통해 서울과 주요 수도권 지역을 규제지역으로 재지정하면서 실수요자들의 자금 흐름이 바뀌고 있다. 투기과열지구와 조정대상지역 확대로 대출</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>공장 신축, 신축공사</t>
+          <t>라인 증설, 증설 공사</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>경북</t>
+          <t>경기도 평택시 합정동</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/011/0004547213?sid=101</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1200,100 +2017,96 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.48194444444</v>
+        <v>45957.12638888889</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>공장 신축, 신축공사</t>
+          <t>공장 증설, 증설 공사</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>경북</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45956.72430555556</v>
+        <v>45956.43819444445</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>인천시 검단6중 신축 현장서 근로자 추락 부상…안전관리 ‘허술’ 지적</t>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>인천광역시 서구 불로동 247-16 일원 에서 추진 중인 가칭 ‘검단6중학교 신축공사’ 현장에서 근로자가 추락해 부상을 입는 사고가 발생했다. 공공 발주 대형 건축사업임에도 기본적</t>
+          <t>(서울=뉴스1) 박기범 기자 = 빌 리 미국 테네시 주지사와 한국앤컴퍼니(000240)그룹이 미국 내 타이어 생산 확대 및 모빌리티 기술 개발을 위한 협력 방안을 모색했다. 한국앤</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>신축공사</t>
+          <t>증설 공사</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>인천광역시 서구 불로동</t>
+          <t>경기도</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/382/0001231641?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008562459?sid=103</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45956.61388888889</v>
+        <v>45954.3875</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>속초시의회, 2025년도 주요사업장 현지답사 실시</t>
+          <t>‘비규제 청정지역’ 평택, 삼성전자 P5 착공 호재에 ‘힐스테이트 평택...</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>속초시의회, 2025년도 주요사업장 현지답사 실시 이번 현지답사는 속초영어도서관 신축공사, 속초시 장애인종합복지센터 조성사업, 속초음식문화복합공간 조성사업 등 시민들의 삶의 질 향</t>
+          <t>[서울경제] 정부가 10·15 부동산 대책을 통해 서울과 주요 수도권 지역을 규제지역으로 재지정하면서 실수요자들의 자금 흐름이 바뀌고 있다. 투기과열지구와 조정대상지역 확대로 대출</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>신축공사</t>
+          <t>라인 증설, 증설 공사</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>경기도 평택시 합정동</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/087/0001150407?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/011/0004547213?sid=101</t>
         </is>
       </c>
     </row>
@@ -1302,13 +2115,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1365,21 +2178,285 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45957.12638888889</v>
+        <v>45957.25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
+          <t>[S리포트] ②'먹튀의 덫'… 산업 동맥경화 부르는 사모펀드식 경영</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
+          <t>"저희는 기업의 가치를 높이는 자본시장의 '메기'입니다." 한때 사모펀드(PEF) 운용사들이 입버릇처럼 하던 말이다. PEF는 본래 저평가된 기업을 인수해 비효율적인 구조를 혁신하</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>공장 증설, 증설 공사</t>
+          <t>시설 투자</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/417/0001108955?sid=101</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45956.38263888889</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>“증권사 앱 설치하는 사이에 50만닉스”…다 놓쳤다면 ‘반도체 5총사...</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>한미반도체·이수페타시스·ISC등 주목 추석 명절 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사가 없는 투자자들은 ‘포모’(FOMO·기회 상실 걱정)가 커진다</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/009/0005579005?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45955.32986111111</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>'아, 포트폴리오 하나쯤 담을 걸'…AI발 훈풍 확산</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>'아, 포트폴리오 하나쯤 담을 걸'…AI발 훈풍 확산 에너지 인프라, 2차전지 관련주에 투자하는 상장지수펀드(ETF)가 이번주 수익률 상위권을 휩쓸었다. 기존 반도체·빅테크 중심으</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2,986</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/215/0001228287?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45954.70555555556</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9만전자·50만닉스 놓쳤다면 …'K반도체 명품조연' 5총사 주목</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>'반도체 투톱' 말고도 AI 수혜 기업들 있다 "삼성전자, SK하이닉스 없어요?" 추석 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사를 보유하지 않은 투자자</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>설비투자</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/009/0005578662?sid=105</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45953.35902777778</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>그로쓰리서치 "인벤티지랩, '균일 미립구'로 장기지속형 시장 정조준"</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 배요한 기자 = 인벤티지랩이 미세유체공학 기반의 제형 플랫폼 'IVL-DrugFluidic'을 앞세워 장기지속형(LAI) 의약품 시장 공략에 속도를 내고 있다. 균</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>공장 투자</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1388,288 +2465,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45956.78541666667</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산 美공장 증설·공급망 재편으로 돌파 넥센, 15%로 완화시 큰 수혜 전망 미국의 관세 폭탄으로 올해 3·4분기 한국타이어앤</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/014/0005424711?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45956.67847222222</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>타이어 3사 3분기 관세 손실 1150억대…공급망 재편으로 돌파구 모색</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">관세 피해에 공급망 재편·가격 인상 대응 관세 15% 인하 시나리오에 업계 기대감 한국타이어의 미국 테네시 공장 전경.사진=한국타이어앤테크놀로지 제공 [파이낸셜뉴스] 미국의 관세 </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/014/0005424606?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45956.48541666667</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹 "美 테네시 주지사와 공동협력 논의"</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>[서울=뉴시스] 류인선 기자 = 한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 경기 판교 본사 테크노플렉스를 방문해 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013557923?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45956.48263888889</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동…“협력 강화 논의”</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 오전 경기도 판교 본사 테크노플렉스를 방문했다고 26일 밝혔다. 리 주지사는 테크노플렉스를 둘러보고, 이수일 부회장 겸 </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>경기도</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/029/0002989234?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45956.47916666666</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>양측은 간담회에서 ▲비즈니스 친화적 환경 조성 ▲원활한 현지 진출을 위한 주정부 차원의 지원 ▲안정적인 에너지 공급 ▲경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005669545?sid=103</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45956.46388888889</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹, 테네시 주지사와 북미 생산·공급망 협력 논의</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>배터리·타이어 공장 증설 등 북미 생산거점 협력 논의 조현범 회장 강조한 ‘국가 경제 기여’ 실현 의지도 재확인 이날 간담회에는 이수일 한국앤컴퍼니그룹 부회장 겸 한온시스템 대표,</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/119/0003016629?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45956.42152777778</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동… 모빌리티 협력 강화</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>이번 방문에서 리 주지사는 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴퍼니 대표이사, 김준현 한국앤컴퍼니 경영총괄, 안종선·이상훈 한국타이어앤테크놀로지 공동대표 등을 만났다</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>6388</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/366/0001117399?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45956.40486111111</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>간담회에서 양측은 △비즈니스 친화적 환경 조성 △원활한 현지 진출을 위한 주정부 차원의 지원 △안정적인 에너지 공급 △경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/008/0005268104?sid=101</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45956.42430555556</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>이번주 공모주 청약, 이노테크 1개사</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>27~28일 공모 청약…내달 7일 코스닥 상장 26일 금융투자업계에 따르면, 이노테크는 오는 27~28일 양일간 일반 공모 청약을 실시한다. 앞서 지난 16일부터 22일까지 수요예</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>공장 증설</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>259</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/119/0003016600?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013552176?sid=101</t>
         </is>
       </c>
     </row>
@@ -1678,7 +2474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1741,63 +2537,1457 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45957.12638888889</v>
+        <v>45954.47083333333</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
+          <t>美 테네시 주지사·한국타이어, 현지투자 협력</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
+          <t>테네시 타이어공장 2조 증설 프로젝트 점검 류진 한경협 회장·이석희 SK온 CEO도 만나 관세 장벽 속 국내 기업과 협력 강화 움직임 6년 만의 방한 일정을 소화 중인 빌 리 테네</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>공장 증설, 증설 공사</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+          <t>신규 투자</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>550만</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/016/0002546811?sid=101</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45956.43819444445</v>
+        <v>45954.38819444444</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+          <t>[단독] 테네시 주지사, 한국타이어 최고경영진과 ‘장시간 회동’…“한...</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(서울=뉴스1) 박기범 기자 = 빌 리 미국 테네시 주지사와 한국앤컴퍼니(000240)그룹이 미국 내 타이어 생산 확대 및 모빌리티 기술 개발을 위한 협력 방안을 모색했다. 한국앤</t>
+          <t>테네시 타이어공장 2조 증설 프로젝트 점검 ‘관세 장벽’ 속 협력 강화 논의 관측 [헤럴드경제(성남)=김성우 기자] 6년 만의 방한 일정을 소화 중인 빌 리 테네시 주지사가 24일</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>증설 공사</t>
+          <t>신규 투자</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>550만</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>경기도 성남시</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/016/0002546648?sid=101</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45954.58819444444</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>증평군-코스맥스펫 400억 규모 신규 공장 설립 투자협약</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(증평=뉴스1) 엄기찬 기자 = 충북 증평군은 코스맥스펫㈜과 증평2일반산업단지에 신규 공장을 설립하는 내용의 투자협약을 했다고 24일 밝혔다. 코스맥스펫은 세계 1위 OEM·ODM</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>투자협약</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>충북 증평군</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008560369?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45954.5875</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>코스맥스펫, 증평2산단 '반려동물 건강식품 공장 ' 설립한다</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[증평=뉴시스] 서주영 기자 = 충북 증평군은 지난 23일 김득신문학관에서 코스맥스펫과 지역 신규 공장을 설립하는 투자협약(MOU)을 체결했다고 24일 밝혔다. 코스맥스펫은 400</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>투자협약</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>충북 증평군</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013555919?sid=102</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45956.96875</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>투자유치, 투자 유치</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/005/0001810151?sid=102</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45956.96875</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>투자유치, 투자 유치</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/005/0001810151?sid=102</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45955.25</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[2025 국정감사] “금융사고 최소화…건전성 관리 강화” 촉구</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>외부인에 의한 사기 피해 증가 지역 농축협 부실대출 등 지적 농협 유통 자회사 경영개선 방안 마사회 퇴역마 보호·지원 주문 ◆농협 금융 건전성 강화 요구 집중=이날 국감에선 농축협</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>공장 신설</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>제주</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/662/0000080587?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45954.25069444445</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"한국판 ASML 필요"…소부장 핵심전략지도 만든다[Pick코노미]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>고부가·탄소중립·핵심광물 등 4대 혁신기술 R&amp;D 역량 집중 15대 프로젝트에 3000억 투자 "첨단산업 기술 수준 83.3점서 2030년 92점까지 끌어올릴것" [서울경제] 정부</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>공장 신설</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/011/0004547151?sid=101</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45956.48194444444</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>공장 신축, 신축공사</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>경북</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45954.725</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>이노테크, 공모가 1만4700원 확정</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11월 7일 코스닥 상장 예정복합 신뢰성 환경시험 장비 전문 기업 이노테크가 공모가를 희망가 상단인 1만 4700원으로 확정했다. 24일 금융투자업계에 따르면 이노테크는 지난 22</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>공장 신축</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>259</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/031/0000974916?sid=101</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45956.48194444444</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>끊이지 않는 작업장 안전사고…경주 질식사고 외 3건 더</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[안동=뉴시스] 류상현 기자 = 경북도내에서 작업장 안전사고가 끊이지 않고 있다. 26일 경북도에 따르면 전날 경주 안강읍 한 공장의 수조에서 작업자 2명이 질식해 숨지고 2명이 </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>공장 신축, 신축공사</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>경북</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013557917?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45954.66875</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"매년 30명 사망"…정부, 내년부터 지붕공사 사고 예방·감독 강화</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>건설업 사망 10%가 지붕공사…봄·가을철 발생 많아 내년부터 대대적 캠페인 후 집중감독…위법 엄중 조치 2027년부터는 건설업 등록업체만 지붕공사 가능 [서울=뉴시스] 고홍주 기자</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>신축공사</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>경기도</t>
+          <t>충남 아산시</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/421/0008562459?sid=103</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013556331?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45956.72430555556</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>인천시 검단6중 신축 현장서 근로자 추락 부상…안전관리 ‘허술’ 지적</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>인천광역시 서구 불로동 247-16 일원 에서 추진 중인 가칭 ‘검단6중학교 신축공사’ 현장에서 근로자가 추락해 부상을 입는 사고가 발생했다. 공공 발주 대형 건축사업임에도 기본적</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>인천광역시 서구 불로동</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/382/0001231641?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45956.61388888889</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>속초시의회, 2025년도 주요사업장 현지답사 실시</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>속초시의회, 2025년도 주요사업장 현지답사 실시 이번 현지답사는 속초영어도서관 신축공사, 속초시 장애인종합복지센터 조성사업, 속초음식문화복합공간 조성사업 등 시민들의 삶의 질 향</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/087/0001150407?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45956.25</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>'싱크홀 경고등' 서울 향후 5년간 10m 이상 지하 굴착 공사 300여곳</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">시 "매달 1회 점검…대형 공사 주1회 집중 점검" (서울=뉴스1) 이비슬 기자 = 향후 5년간 서울 전역에서 땅속 10m 이상을 굴착하는 공사 현장이 300여곳에 이르는 것으로 </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008562260?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45954.85833333333</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013556752?sid=100</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45954.85833333333</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013556750?sid=100</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45954.85833333333</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013556751?sid=100</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45954.85833333333</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>김영훈 노동부 장관, 공사 현장 안전관리 실태 점검</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 김영훈 고용노동부 장관이 24일 충남 아산시 물류창고 신축공사 현장을 찾아 추락사고 예방 등 안전관리 실태를 확인하고 있다. (사진=고용노동부 제공) 2025.10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>신축공사</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>충남 아산시</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013556753?sid=100</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>게재시각(KST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>헤드라인</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>내용요약</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>규모</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>투자금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>공사지역</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>담당자 연락처</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>원본기사 URL 링크</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45954.53541666667</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>조현준 효성그룹 회장 "글로벌 수요 대응 위해선 생산능력 확보 필수"</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">조현준 효성그룹 회장 "글로벌 수요 대응 위해선 생산능력 확보 필수" 효성중공업이 국내외 생산거점 가동률 역대 최고 수준을 기록하며 '글로벌 전력기기 시장'에서 존재감을 강화하고 </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2071</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>경남</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/047/0002492510?sid=100</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45957.12638888889</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니, 美테네시 주지사 회동 ‘북미 사업 강화’ 한국앤컴퍼니그룹은 빌 리 테네시 주지사가 24일 오전 경기 성남시 판교 한국앤컴퍼니그룹 본사 테크노플렉스를 방문해 이수일 부</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>공장 증설, 증설 공사</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/020/0003669810?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45956.78541666667</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>‘관세 폭탄’ 타이어 3사, 3분기 1150억대 손실 추산 美공장 증설·공급망 재편으로 돌파 넥센, 15%로 완화시 큰 수혜 전망 미국의 관세 폭탄으로 올해 3·4분기 한국타이어앤</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/014/0005424711?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45956.67847222222</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>타이어 3사 3분기 관세 손실 1150억대…공급망 재편으로 돌파구 모색</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관세 피해에 공급망 재편·가격 인상 대응 관세 15% 인하 시나리오에 업계 기대감 한국타이어의 미국 테네시 공장 전경.사진=한국타이어앤테크놀로지 제공 [파이낸셜뉴스] 미국의 관세 </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/014/0005424606?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45956.48541666667</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹 "美 테네시 주지사와 공동협력 논의"</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[서울=뉴시스] 류인선 기자 = 한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 경기 판교 본사 테크노플렉스를 방문해 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013557923?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45956.48263888889</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동…“협력 강화 논의”</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">한국앤컴퍼니그룹은 빌 리 미국 테네시 주지사가 지난 24일 오전 경기도 판교 본사 테크노플렉스를 방문했다고 26일 밝혔다. 리 주지사는 테크노플렉스를 둘러보고, 이수일 부회장 겸 </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>경기도</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/029/0002989234?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45956.47916666666</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>양측은 간담회에서 ▲비즈니스 친화적 환경 조성 ▲원활한 현지 진출을 위한 주정부 차원의 지원 ▲안정적인 에너지 공급 ▲경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/277/0005669545?sid=103</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45956.46388888889</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 테네시 주지사와 북미 생산·공급망 협력 논의</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>배터리·타이어 공장 증설 등 북미 생산거점 협력 논의 조현범 회장 강조한 ‘국가 경제 기여’ 실현 의지도 재확인 이날 간담회에는 이수일 한국앤컴퍼니그룹 부회장 겸 한온시스템 대표,</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/119/0003016629?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45956.42152777778</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동… 모빌리티 협력 강화</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>이번 방문에서 리 주지사는 이수일 부회장 겸 한온시스템 대표, 박종호 한국앤컴퍼니 대표이사, 김준현 한국앤컴퍼니 경영총괄, 안종선·이상훈 한국타이어앤테크놀로지 공동대표 등을 만났다</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/366/0001117399?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45956.40486111111</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>한국앤컴퍼니그룹, 美 테네시 주지사 회동 "지원·협력 강화"</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>간담회에서 양측은 △비즈니스 친화적 환경 조성 △원활한 현지 진출을 위한 주정부 차원의 지원 △안정적인 에너지 공급 △경쟁력 있는 현지 인력 확보 등 모빌리티 산업 발전 협력 강화</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/008/0005268104?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45956.42430555556</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>이번주 공모주 청약, 이노테크 1개사</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>27~28일 공모 청약…내달 7일 코스닥 상장 26일 금융투자업계에 따르면, 이노테크는 오는 27~28일 양일간 일반 공모 청약을 실시한다. 앞서 지난 16일부터 22일까지 수요예</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>공장 증설</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>259</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/119/0003016600?sid=101</t>
         </is>
       </c>
     </row>
@@ -1869,34 +4059,34 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45957.25</v>
+        <v>45952.6875</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[S리포트] ②'먹튀의 덫'… 산업 동맥경화 부르는 사모펀드식 경영</t>
+          <t>LS일렉, 3분기 영업익 1007억…작년 동기 대비 51.7%↑</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"저희는 기업의 가치를 높이는 자본시장의 '메기'입니다." 한때 사모펀드(PEF) 운용사들이 입버릇처럼 하던 말이다. PEF는 본래 저평가된 기업을 인수해 비효율적인 구조를 혁신하</t>
+          <t>(서울=뉴스1) 원태성 기자 = LS일렉트릭이 인공지능(AI) 시대 전력기기 호황에 힘입어 3분기 영업이익이 50% 이상 급증하고 매출 역시 20% 가까이 늘어났다. LS일렉트릭은</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>시설 투자</t>
+          <t>생산능력 확대</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1007</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/417/0001108955?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008555777?sid=101</t>
         </is>
       </c>
     </row>
@@ -1968,34 +4158,34 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.38263888889</v>
+        <v>45952.66944444444</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>“증권사 앱 설치하는 사이에 50만닉스”…다 놓쳤다면 ‘반도체 5총사...</t>
+          <t>LS일렉트릭, 실적 훈풍 제대로 탔다…북미 수주 물밀듯</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>한미반도체·이수페타시스·ISC등 주목 추석 명절 이후에도 K반도체 주식 유무에 대한 질문이 끊이지 않는다. 두 상장사가 없는 투자자들은 ‘포모’(FOMO·기회 상실 걱정)가 커진다</t>
+          <t>북미 매출 비중 33%·5년간 연평균 성장률 50% 달해 자동화 흑자전환·자회사 호조로 수익성 개선세 강화 수주잔고 4.1조 '사상 최대' LS일렉트릭은 올해 3분기 연결기준 매출</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>설비투자</t>
+          <t>공장 증축</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2162</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/009/0005579005?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/648/0000040955?sid=101</t>
         </is>
       </c>
     </row>
@@ -2010,7 +4200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2067,34 +4257,129 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.96875</v>
+        <v>45955.40694444445</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+          <t>[자막뉴스] " 공사 소리도 좋아"...'3억 달러' 무도회장 착공 논란 파장 ...</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+          <t>[자막뉴스] "공사 소리도 좋아"...'3억 달러' 무도회장 착공 논란 파장 계속 수용 인원 999명의 대형 무도회장 신축 공사가 시작됐습니다. [도널드 트럼프 / 미국 대통령 :</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>투자유치, 투자 유치</t>
+          <t>증축 공사</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>경기도</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>02-398-8585</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/005/0001810151?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/052/0002264247?sid=104</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45955.10138888889</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>백악관에 '3억 달러' 무도회장 착공...불투명 지적에 트럼프 "3류 기자"</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>백악관에 '3억 달러' 무도회장 착공...불투명 지적에 트럼프 "3류 기자" 미국 연방정부의 일시적 업무중지, '셧다운'이 20여 일째 이어지는 가운데 백악관에서는 3억 달러가 들</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>증축 공사</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>02-398-8585</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/052/0002264171?sid=104</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45955.53958333333</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>조승환 의원, 혜광고 다목적강당 증축 …교육부 특별교부금 18.8억 확보</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(부산=뉴스1) 임순택 기자 = 조승환 국민의힘 의원(부산 중구·영도구)이 부산 혜광고등학교 다목적강당 증축 사업을 위한 교육부 특별교부금 18억 8100만 원을 확보했다고 25일</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>증축 공사, 증축공사</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008561885?sid=102</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45954.73263888889</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>정부 부채만 38조 달러인데…백악관 뜯어고치는 트럼프</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">'건물 철거 안 해' 약속 파기 정부 계약 체결 기업 기부금 논란 도널드 트럼프 미국 대통령이 추진하는 백악관 증축 공사에 논란이 일고 있다. 1902년 건설된 이스트윙(동관)을 </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>증축 공사</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1433</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/629/0000437186?sid=104</t>
         </is>
       </c>
     </row>
@@ -2166,34 +4451,30 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.96875</v>
+        <v>45955.53958333333</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>김동연 “기후위기, 기회로 바꾸는 기후경제 필요한 시대” 강조 이유 ...</t>
+          <t>조승환 의원, 혜광고 다목적강당 증축 …교육부 특별교부금 18.8억 확보</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>김동연 경기도지사가 “기후위기를 기회로 바꾸는 기후경제가 필요한 시대”라고 강조하고 나섰다. 김 지사는 지난 24일 수원 경기융합타운(경기신용보증재단 3층)에서 열린 ‘2025 경</t>
+          <t>(부산=뉴스1) 임순택 기자 = 조승환 국민의힘 의원(부산 중구·영도구)이 부산 혜광고등학교 다목적강당 증축 사업을 위한 교육부 특별교부금 18억 8100만 원을 확보했다고 25일</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>투자유치, 투자 유치</t>
+          <t>증축 공사, 증축공사</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>경기도</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/005/0001810151?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008561885?sid=102</t>
         </is>
       </c>
     </row>

</xml_diff>